<commit_message>
Updated Gantt Chart. Renamed and organized levels. Moved old designs into prefabs to save on graphics rendering.
</commit_message>
<xml_diff>
--- a/Documents/Simple Gantt Chart1.xlsx
+++ b/Documents/Simple Gantt Chart1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeym\lmu\lmu-cmsi-401\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\School Related\CMSI\CMSI 401\Interrobang\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{20FBEDBD-61EC-4E3F-A63C-AFCE29EFD6C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <definedName name="task_start" localSheetId="0">ProjectSchedule!$E1</definedName>
     <definedName name="today" localSheetId="0">TODAY()</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,12 +34,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="H6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -363,7 +362,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
@@ -1000,6 +999,39 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="12" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="10" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1008,9 +1040,6 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
@@ -1022,54 +1051,24 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="10" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Date" xfId="10" xr:uid="{229918B6-DD13-4F5A-97B9-305F7E002AA3}"/>
+    <cellStyle name="Date" xfId="10"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Name" xfId="11" xr:uid="{B2D3C1EE-6B41-4801-AAFC-C2274E49E503}"/>
+    <cellStyle name="Name" xfId="11"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="Project Start" xfId="9" xr:uid="{8EB8A09A-C31C-40A3-B2C1-9449520178B8}"/>
-    <cellStyle name="Task" xfId="12" xr:uid="{6391D789-272B-4DD2-9BF3-2CDCF610FA41}"/>
+    <cellStyle name="Project Start" xfId="9"/>
+    <cellStyle name="Task" xfId="12"/>
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
+    <cellStyle name="zHiddenText" xfId="3"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -1197,7 +1196,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="ToDoList" pivot="0" count="9">
       <tableStyleElement type="wholeTable" dxfId="11"/>
       <tableStyleElement type="headerRow" dxfId="10"/>
       <tableStyleElement type="totalRow" dxfId="9"/>
@@ -1320,7 +1319,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1617,15 +1616,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:DI47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1660,7 +1659,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="65"/>
-      <c r="I2" s="96"/>
+      <c r="I2" s="88"/>
     </row>
     <row r="3" spans="1:113" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
@@ -1669,187 +1668,187 @@
       <c r="B3" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="85">
+      <c r="D3" s="93"/>
+      <c r="E3" s="95">
         <v>43355</v>
       </c>
-      <c r="F3" s="81"/>
+      <c r="F3" s="96"/>
     </row>
     <row r="4" spans="1:113" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="83"/>
+      <c r="D4" s="93"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="78">
+      <c r="I4" s="89">
         <f>I5</f>
         <v>43353</v>
       </c>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="80"/>
-      <c r="P4" s="78">
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="89">
         <f>P5</f>
         <v>43360</v>
       </c>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="79"/>
-      <c r="S4" s="79"/>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="80"/>
-      <c r="W4" s="78">
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="91"/>
+      <c r="W4" s="89">
         <f>W5</f>
         <v>43367</v>
       </c>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="79"/>
-      <c r="Z4" s="79"/>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="80"/>
-      <c r="AD4" s="78">
+      <c r="X4" s="90"/>
+      <c r="Y4" s="90"/>
+      <c r="Z4" s="90"/>
+      <c r="AA4" s="90"/>
+      <c r="AB4" s="90"/>
+      <c r="AC4" s="91"/>
+      <c r="AD4" s="89">
         <f>AD5</f>
         <v>43374</v>
       </c>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="79"/>
-      <c r="AG4" s="79"/>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="80"/>
-      <c r="AK4" s="78">
+      <c r="AE4" s="90"/>
+      <c r="AF4" s="90"/>
+      <c r="AG4" s="90"/>
+      <c r="AH4" s="90"/>
+      <c r="AI4" s="90"/>
+      <c r="AJ4" s="91"/>
+      <c r="AK4" s="89">
         <f>AK5</f>
         <v>43381</v>
       </c>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="79"/>
-      <c r="AN4" s="79"/>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="80"/>
-      <c r="AR4" s="78">
+      <c r="AL4" s="90"/>
+      <c r="AM4" s="90"/>
+      <c r="AN4" s="90"/>
+      <c r="AO4" s="90"/>
+      <c r="AP4" s="90"/>
+      <c r="AQ4" s="91"/>
+      <c r="AR4" s="89">
         <f>AR5</f>
         <v>43388</v>
       </c>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="79"/>
-      <c r="AU4" s="79"/>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="80"/>
-      <c r="AY4" s="78">
+      <c r="AS4" s="90"/>
+      <c r="AT4" s="90"/>
+      <c r="AU4" s="90"/>
+      <c r="AV4" s="90"/>
+      <c r="AW4" s="90"/>
+      <c r="AX4" s="91"/>
+      <c r="AY4" s="89">
         <f>AY5</f>
         <v>43395</v>
       </c>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="79"/>
-      <c r="BB4" s="79"/>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="80"/>
-      <c r="BF4" s="78">
+      <c r="AZ4" s="90"/>
+      <c r="BA4" s="90"/>
+      <c r="BB4" s="90"/>
+      <c r="BC4" s="90"/>
+      <c r="BD4" s="90"/>
+      <c r="BE4" s="91"/>
+      <c r="BF4" s="89">
         <f>BF5</f>
         <v>43402</v>
       </c>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="79"/>
-      <c r="BI4" s="79"/>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="80"/>
-      <c r="BM4" s="78">
+      <c r="BG4" s="90"/>
+      <c r="BH4" s="90"/>
+      <c r="BI4" s="90"/>
+      <c r="BJ4" s="90"/>
+      <c r="BK4" s="90"/>
+      <c r="BL4" s="91"/>
+      <c r="BM4" s="89">
         <f>BM5</f>
         <v>43409</v>
       </c>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="79"/>
-      <c r="BP4" s="79"/>
-      <c r="BQ4" s="79"/>
-      <c r="BR4" s="79"/>
-      <c r="BS4" s="80"/>
-      <c r="BT4" s="78">
+      <c r="BN4" s="90"/>
+      <c r="BO4" s="90"/>
+      <c r="BP4" s="90"/>
+      <c r="BQ4" s="90"/>
+      <c r="BR4" s="90"/>
+      <c r="BS4" s="91"/>
+      <c r="BT4" s="89">
         <f>BT5</f>
         <v>43416</v>
       </c>
-      <c r="BU4" s="79"/>
-      <c r="BV4" s="79"/>
-      <c r="BW4" s="79"/>
-      <c r="BX4" s="79"/>
-      <c r="BY4" s="79"/>
-      <c r="BZ4" s="80"/>
-      <c r="CA4" s="78">
+      <c r="BU4" s="90"/>
+      <c r="BV4" s="90"/>
+      <c r="BW4" s="90"/>
+      <c r="BX4" s="90"/>
+      <c r="BY4" s="90"/>
+      <c r="BZ4" s="91"/>
+      <c r="CA4" s="89">
         <f>CA5</f>
         <v>43423</v>
       </c>
-      <c r="CB4" s="79"/>
-      <c r="CC4" s="79"/>
-      <c r="CD4" s="79"/>
-      <c r="CE4" s="79"/>
-      <c r="CF4" s="79"/>
-      <c r="CG4" s="80"/>
-      <c r="CH4" s="78">
+      <c r="CB4" s="90"/>
+      <c r="CC4" s="90"/>
+      <c r="CD4" s="90"/>
+      <c r="CE4" s="90"/>
+      <c r="CF4" s="90"/>
+      <c r="CG4" s="91"/>
+      <c r="CH4" s="89">
         <f>CH5</f>
         <v>43430</v>
       </c>
-      <c r="CI4" s="79"/>
-      <c r="CJ4" s="79"/>
-      <c r="CK4" s="79"/>
-      <c r="CL4" s="79"/>
-      <c r="CM4" s="79"/>
-      <c r="CN4" s="80"/>
-      <c r="CO4" s="78">
+      <c r="CI4" s="90"/>
+      <c r="CJ4" s="90"/>
+      <c r="CK4" s="90"/>
+      <c r="CL4" s="90"/>
+      <c r="CM4" s="90"/>
+      <c r="CN4" s="91"/>
+      <c r="CO4" s="89">
         <f>CO5</f>
         <v>43437</v>
       </c>
-      <c r="CP4" s="79"/>
-      <c r="CQ4" s="79"/>
-      <c r="CR4" s="79"/>
-      <c r="CS4" s="79"/>
-      <c r="CT4" s="79"/>
-      <c r="CU4" s="80"/>
-      <c r="CV4" s="78">
+      <c r="CP4" s="90"/>
+      <c r="CQ4" s="90"/>
+      <c r="CR4" s="90"/>
+      <c r="CS4" s="90"/>
+      <c r="CT4" s="90"/>
+      <c r="CU4" s="91"/>
+      <c r="CV4" s="89">
         <f>CV5</f>
         <v>43444</v>
       </c>
-      <c r="CW4" s="79"/>
-      <c r="CX4" s="79"/>
-      <c r="CY4" s="79"/>
-      <c r="CZ4" s="79"/>
-      <c r="DA4" s="79"/>
-      <c r="DB4" s="80"/>
-      <c r="DC4" s="78">
+      <c r="CW4" s="90"/>
+      <c r="CX4" s="90"/>
+      <c r="CY4" s="90"/>
+      <c r="CZ4" s="90"/>
+      <c r="DA4" s="90"/>
+      <c r="DB4" s="91"/>
+      <c r="DC4" s="89">
         <f>DC5</f>
         <v>43451</v>
       </c>
-      <c r="DD4" s="79"/>
-      <c r="DE4" s="79"/>
-      <c r="DF4" s="79"/>
-      <c r="DG4" s="79"/>
-      <c r="DH4" s="79"/>
-      <c r="DI4" s="80"/>
+      <c r="DD4" s="90"/>
+      <c r="DE4" s="90"/>
+      <c r="DF4" s="90"/>
+      <c r="DG4" s="90"/>
+      <c r="DH4" s="90"/>
+      <c r="DI4" s="91"/>
     </row>
     <row r="5" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43353</v>
@@ -2047,227 +2046,227 @@
         <v>43401</v>
       </c>
       <c r="BF5" s="11">
-        <f>BE5+1</f>
+        <f t="shared" ref="BF5:CK5" si="2">BE5+1</f>
         <v>43402</v>
       </c>
       <c r="BG5" s="10">
-        <f>BF5+1</f>
+        <f t="shared" si="2"/>
         <v>43403</v>
       </c>
       <c r="BH5" s="10">
-        <f>BG5+1</f>
+        <f t="shared" si="2"/>
         <v>43404</v>
       </c>
       <c r="BI5" s="10">
-        <f>BH5+1</f>
+        <f t="shared" si="2"/>
         <v>43405</v>
       </c>
       <c r="BJ5" s="10">
-        <f>BI5+1</f>
+        <f t="shared" si="2"/>
         <v>43406</v>
       </c>
       <c r="BK5" s="10">
-        <f>BJ5+1</f>
+        <f t="shared" si="2"/>
         <v>43407</v>
       </c>
       <c r="BL5" s="12">
-        <f>BK5+1</f>
+        <f t="shared" si="2"/>
         <v>43408</v>
       </c>
       <c r="BM5" s="11">
-        <f>BL5+1</f>
+        <f t="shared" si="2"/>
         <v>43409</v>
       </c>
       <c r="BN5" s="10">
-        <f>BM5+1</f>
+        <f t="shared" si="2"/>
         <v>43410</v>
       </c>
       <c r="BO5" s="10">
-        <f>BN5+1</f>
+        <f t="shared" si="2"/>
         <v>43411</v>
       </c>
       <c r="BP5" s="10">
-        <f>BO5+1</f>
+        <f t="shared" si="2"/>
         <v>43412</v>
       </c>
       <c r="BQ5" s="10">
-        <f>BP5+1</f>
+        <f t="shared" si="2"/>
         <v>43413</v>
       </c>
       <c r="BR5" s="10">
-        <f>BQ5+1</f>
+        <f t="shared" si="2"/>
         <v>43414</v>
       </c>
       <c r="BS5" s="12">
-        <f>BR5+1</f>
+        <f t="shared" si="2"/>
         <v>43415</v>
       </c>
       <c r="BT5" s="11">
-        <f>BS5+1</f>
+        <f t="shared" si="2"/>
         <v>43416</v>
       </c>
       <c r="BU5" s="10">
-        <f>BT5+1</f>
+        <f t="shared" si="2"/>
         <v>43417</v>
       </c>
       <c r="BV5" s="10">
-        <f>BU5+1</f>
+        <f t="shared" si="2"/>
         <v>43418</v>
       </c>
       <c r="BW5" s="10">
-        <f>BV5+1</f>
+        <f t="shared" si="2"/>
         <v>43419</v>
       </c>
       <c r="BX5" s="10">
-        <f>BW5+1</f>
+        <f t="shared" si="2"/>
         <v>43420</v>
       </c>
       <c r="BY5" s="10">
-        <f>BX5+1</f>
+        <f t="shared" si="2"/>
         <v>43421</v>
       </c>
       <c r="BZ5" s="12">
-        <f>BY5+1</f>
+        <f t="shared" si="2"/>
         <v>43422</v>
       </c>
       <c r="CA5" s="11">
-        <f>BZ5+1</f>
+        <f t="shared" si="2"/>
         <v>43423</v>
       </c>
       <c r="CB5" s="10">
-        <f>CA5+1</f>
+        <f t="shared" si="2"/>
         <v>43424</v>
       </c>
       <c r="CC5" s="10">
-        <f>CB5+1</f>
+        <f t="shared" si="2"/>
         <v>43425</v>
       </c>
       <c r="CD5" s="10">
-        <f>CC5+1</f>
+        <f t="shared" si="2"/>
         <v>43426</v>
       </c>
       <c r="CE5" s="10">
-        <f>CD5+1</f>
+        <f t="shared" si="2"/>
         <v>43427</v>
       </c>
       <c r="CF5" s="10">
-        <f>CE5+1</f>
+        <f t="shared" si="2"/>
         <v>43428</v>
       </c>
       <c r="CG5" s="12">
-        <f>CF5+1</f>
+        <f t="shared" si="2"/>
         <v>43429</v>
       </c>
       <c r="CH5" s="11">
-        <f>CG5+1</f>
+        <f t="shared" si="2"/>
         <v>43430</v>
       </c>
       <c r="CI5" s="10">
-        <f>CH5+1</f>
+        <f t="shared" si="2"/>
         <v>43431</v>
       </c>
       <c r="CJ5" s="10">
-        <f>CI5+1</f>
+        <f t="shared" si="2"/>
         <v>43432</v>
       </c>
       <c r="CK5" s="10">
-        <f>CJ5+1</f>
+        <f t="shared" si="2"/>
         <v>43433</v>
       </c>
       <c r="CL5" s="10">
-        <f>CK5+1</f>
+        <f t="shared" ref="CL5:DI5" si="3">CK5+1</f>
         <v>43434</v>
       </c>
       <c r="CM5" s="10">
-        <f>CL5+1</f>
+        <f t="shared" si="3"/>
         <v>43435</v>
       </c>
       <c r="CN5" s="12">
-        <f>CM5+1</f>
+        <f t="shared" si="3"/>
         <v>43436</v>
       </c>
       <c r="CO5" s="11">
-        <f>CN5+1</f>
+        <f t="shared" si="3"/>
         <v>43437</v>
       </c>
       <c r="CP5" s="10">
-        <f>CO5+1</f>
+        <f t="shared" si="3"/>
         <v>43438</v>
       </c>
       <c r="CQ5" s="10">
-        <f>CP5+1</f>
+        <f t="shared" si="3"/>
         <v>43439</v>
       </c>
       <c r="CR5" s="10">
-        <f>CQ5+1</f>
+        <f t="shared" si="3"/>
         <v>43440</v>
       </c>
       <c r="CS5" s="10">
-        <f>CR5+1</f>
+        <f t="shared" si="3"/>
         <v>43441</v>
       </c>
       <c r="CT5" s="10">
-        <f>CS5+1</f>
+        <f t="shared" si="3"/>
         <v>43442</v>
       </c>
       <c r="CU5" s="12">
-        <f>CT5+1</f>
+        <f t="shared" si="3"/>
         <v>43443</v>
       </c>
       <c r="CV5" s="11">
-        <f>CU5+1</f>
+        <f t="shared" si="3"/>
         <v>43444</v>
       </c>
       <c r="CW5" s="10">
-        <f>CV5+1</f>
+        <f t="shared" si="3"/>
         <v>43445</v>
       </c>
       <c r="CX5" s="10">
-        <f>CW5+1</f>
+        <f t="shared" si="3"/>
         <v>43446</v>
       </c>
       <c r="CY5" s="10">
-        <f>CX5+1</f>
+        <f t="shared" si="3"/>
         <v>43447</v>
       </c>
       <c r="CZ5" s="10">
-        <f>CY5+1</f>
+        <f t="shared" si="3"/>
         <v>43448</v>
       </c>
       <c r="DA5" s="10">
-        <f>CZ5+1</f>
+        <f t="shared" si="3"/>
         <v>43449</v>
       </c>
       <c r="DB5" s="12">
-        <f>DA5+1</f>
+        <f t="shared" si="3"/>
         <v>43450</v>
       </c>
       <c r="DC5" s="11">
-        <f>DB5+1</f>
+        <f t="shared" si="3"/>
         <v>43451</v>
       </c>
       <c r="DD5" s="10">
-        <f>DC5+1</f>
+        <f t="shared" si="3"/>
         <v>43452</v>
       </c>
       <c r="DE5" s="10">
-        <f>DD5+1</f>
+        <f t="shared" si="3"/>
         <v>43453</v>
       </c>
       <c r="DF5" s="10">
-        <f>DE5+1</f>
+        <f t="shared" si="3"/>
         <v>43454</v>
       </c>
       <c r="DG5" s="10">
-        <f>DF5+1</f>
+        <f t="shared" si="3"/>
         <v>43455</v>
       </c>
       <c r="DH5" s="10">
-        <f>DG5+1</f>
+        <f t="shared" si="3"/>
         <v>43456</v>
       </c>
       <c r="DI5" s="12">
-        <f>DH5+1</f>
+        <f t="shared" si="3"/>
         <v>43457</v>
       </c>
     </row>
@@ -2295,199 +2294,199 @@
         <v>7</v>
       </c>
       <c r="I6" s="13" t="str">
-        <f t="shared" ref="I6" si="2">LEFT(TEXT(I5,"ddd"),1)</f>
+        <f t="shared" ref="I6" si="4">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
       </c>
       <c r="J6" s="13" t="str">
-        <f t="shared" ref="J6:AR6" si="3">LEFT(TEXT(J5,"ddd"),1)</f>
+        <f t="shared" ref="J6:AR6" si="5">LEFT(TEXT(J5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="K6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>W</v>
       </c>
       <c r="L6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>T</v>
       </c>
       <c r="M6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>F</v>
       </c>
       <c r="N6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="O6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="P6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>M</v>
       </c>
       <c r="Q6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>T</v>
       </c>
       <c r="R6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>W</v>
       </c>
       <c r="S6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>T</v>
       </c>
       <c r="T6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>F</v>
       </c>
       <c r="U6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="V6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="W6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>M</v>
       </c>
       <c r="X6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>T</v>
       </c>
       <c r="Y6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>W</v>
       </c>
       <c r="Z6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>T</v>
       </c>
       <c r="AA6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>F</v>
       </c>
       <c r="AB6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="AC6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="AD6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>M</v>
       </c>
       <c r="AE6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>T</v>
       </c>
       <c r="AF6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>W</v>
       </c>
       <c r="AG6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>T</v>
       </c>
       <c r="AH6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>F</v>
       </c>
       <c r="AI6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="AJ6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="AK6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>M</v>
       </c>
       <c r="AL6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>T</v>
       </c>
       <c r="AM6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>W</v>
       </c>
       <c r="AN6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>T</v>
       </c>
       <c r="AO6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>F</v>
       </c>
       <c r="AP6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="AQ6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="AR6" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>M</v>
       </c>
       <c r="AS6" s="13" t="str">
-        <f t="shared" ref="AS6:BL6" si="4">LEFT(TEXT(AS5,"ddd"),1)</f>
+        <f t="shared" ref="AS6:BL6" si="6">LEFT(TEXT(AS5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="AT6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>W</v>
       </c>
       <c r="AU6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>T</v>
       </c>
       <c r="AV6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>F</v>
       </c>
       <c r="AW6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="AX6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="AY6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>M</v>
       </c>
       <c r="AZ6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>T</v>
       </c>
       <c r="BA6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>W</v>
       </c>
       <c r="BB6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>T</v>
       </c>
       <c r="BC6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>F</v>
       </c>
       <c r="BD6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="BE6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="BF6" s="13" t="str">
@@ -2495,27 +2494,27 @@
         <v>M</v>
       </c>
       <c r="BG6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>T</v>
       </c>
       <c r="BH6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>W</v>
       </c>
       <c r="BI6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>T</v>
       </c>
       <c r="BJ6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>F</v>
       </c>
       <c r="BK6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="BL6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>S</v>
       </c>
       <c r="BM6" s="13" t="str">
@@ -2523,27 +2522,27 @@
         <v>M</v>
       </c>
       <c r="BN6" s="13" t="str">
-        <f t="shared" ref="BN6:BS6" si="5">LEFT(TEXT(BN5,"ddd"),1)</f>
+        <f t="shared" ref="BN6:BS6" si="7">LEFT(TEXT(BN5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="BO6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>W</v>
       </c>
       <c r="BP6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>T</v>
       </c>
       <c r="BQ6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>F</v>
       </c>
       <c r="BR6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>S</v>
       </c>
       <c r="BS6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>S</v>
       </c>
       <c r="BT6" s="13" t="str">
@@ -2551,27 +2550,27 @@
         <v>M</v>
       </c>
       <c r="BU6" s="13" t="str">
-        <f t="shared" ref="BU6:BZ6" si="6">LEFT(TEXT(BU5,"ddd"),1)</f>
+        <f t="shared" ref="BU6:BZ6" si="8">LEFT(TEXT(BU5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="BV6" s="13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>W</v>
       </c>
       <c r="BW6" s="13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>T</v>
       </c>
       <c r="BX6" s="13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>F</v>
       </c>
       <c r="BY6" s="13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>S</v>
       </c>
       <c r="BZ6" s="13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>S</v>
       </c>
       <c r="CA6" s="13" t="str">
@@ -2579,27 +2578,27 @@
         <v>M</v>
       </c>
       <c r="CB6" s="13" t="str">
-        <f t="shared" ref="CB6:CG6" si="7">LEFT(TEXT(CB5,"ddd"),1)</f>
+        <f t="shared" ref="CB6:CG6" si="9">LEFT(TEXT(CB5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="CC6" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>W</v>
       </c>
       <c r="CD6" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
       <c r="CE6" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>F</v>
       </c>
       <c r="CF6" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
       <c r="CG6" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
       <c r="CH6" s="13" t="str">
@@ -2607,27 +2606,27 @@
         <v>M</v>
       </c>
       <c r="CI6" s="13" t="str">
-        <f t="shared" ref="CI6:CN6" si="8">LEFT(TEXT(CI5,"ddd"),1)</f>
+        <f t="shared" ref="CI6:CN6" si="10">LEFT(TEXT(CI5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="CJ6" s="13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>W</v>
       </c>
       <c r="CK6" s="13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>T</v>
       </c>
       <c r="CL6" s="13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>F</v>
       </c>
       <c r="CM6" s="13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
       <c r="CN6" s="13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
       <c r="CO6" s="13" t="str">
@@ -2635,27 +2634,27 @@
         <v>M</v>
       </c>
       <c r="CP6" s="13" t="str">
-        <f t="shared" ref="CP6:CU6" si="9">LEFT(TEXT(CP5,"ddd"),1)</f>
+        <f t="shared" ref="CP6:CU6" si="11">LEFT(TEXT(CP5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="CQ6" s="13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>W</v>
       </c>
       <c r="CR6" s="13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>T</v>
       </c>
       <c r="CS6" s="13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>F</v>
       </c>
       <c r="CT6" s="13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>S</v>
       </c>
       <c r="CU6" s="13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>S</v>
       </c>
       <c r="CV6" s="13" t="str">
@@ -2663,27 +2662,27 @@
         <v>M</v>
       </c>
       <c r="CW6" s="13" t="str">
-        <f t="shared" ref="CW6:DB6" si="10">LEFT(TEXT(CW5,"ddd"),1)</f>
+        <f t="shared" ref="CW6:DB6" si="12">LEFT(TEXT(CW5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="CX6" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>W</v>
       </c>
       <c r="CY6" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>T</v>
       </c>
       <c r="CZ6" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>F</v>
       </c>
       <c r="DA6" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>S</v>
       </c>
       <c r="DB6" s="13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>S</v>
       </c>
       <c r="DC6" s="13" t="str">
@@ -2691,27 +2690,27 @@
         <v>M</v>
       </c>
       <c r="DD6" s="13" t="str">
-        <f t="shared" ref="DD6:DI6" si="11">LEFT(TEXT(DD5,"ddd"),1)</f>
+        <f t="shared" ref="DD6:DI6" si="13">LEFT(TEXT(DD5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="DE6" s="13" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>W</v>
       </c>
       <c r="DF6" s="13" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>T</v>
       </c>
       <c r="DG6" s="13" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>F</v>
       </c>
       <c r="DH6" s="13" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>S</v>
       </c>
       <c r="DI6" s="13" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>S</v>
       </c>
     </row>
@@ -2844,7 +2843,7 @@
       <c r="F8" s="21"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17" t="str">
-        <f t="shared" ref="H8:H44" si="12">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H44" si="14">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="44"/>
@@ -2957,10 +2956,10 @@
       <c r="A9" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="79" t="s">
         <v>43</v>
       </c>
       <c r="D9" s="22">
@@ -2975,7 +2974,7 @@
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="I9" s="44"/>
@@ -3088,14 +3087,14 @@
       <c r="A10" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="87" t="s">
+      <c r="C10" s="79" t="s">
         <v>45</v>
       </c>
       <c r="D10" s="22">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E10" s="67">
         <v>43364</v>
@@ -3106,7 +3105,7 @@
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="I10" s="44"/>
@@ -3217,14 +3216,14 @@
     </row>
     <row r="11" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="60"/>
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="87" t="s">
+      <c r="C11" s="79" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="22">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="E11" s="67">
         <v>43364</v>
@@ -3235,7 +3234,7 @@
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>11</v>
       </c>
       <c r="I11" s="44"/>
@@ -3346,10 +3345,10 @@
     </row>
     <row r="12" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="60"/>
-      <c r="B12" s="86" t="s">
+      <c r="B12" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="87" t="s">
+      <c r="C12" s="79" t="s">
         <v>50</v>
       </c>
       <c r="D12" s="22">
@@ -3363,7 +3362,7 @@
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="I12" s="44"/>
@@ -3474,10 +3473,10 @@
     </row>
     <row r="13" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="60"/>
-      <c r="B13" s="86" t="s">
+      <c r="B13" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="87" t="s">
+      <c r="C13" s="79" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="22">
@@ -3599,14 +3598,14 @@
     </row>
     <row r="14" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="60"/>
-      <c r="B14" s="86" t="s">
+      <c r="B14" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="C14" s="87" t="s">
+      <c r="C14" s="79" t="s">
         <v>49</v>
       </c>
       <c r="D14" s="22">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E14" s="67">
         <v>43369</v>
@@ -3616,7 +3615,7 @@
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="I14" s="44"/>
@@ -3736,7 +3735,7 @@
       <c r="F15" s="26"/>
       <c r="G15" s="17"/>
       <c r="H15" s="17" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I15" s="44"/>
@@ -3849,10 +3848,10 @@
       <c r="A16" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="88" t="s">
+      <c r="B16" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="89" t="s">
+      <c r="C16" s="81" t="s">
         <v>58</v>
       </c>
       <c r="D16" s="27">
@@ -3866,7 +3865,7 @@
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="I16" s="44"/>
@@ -3977,10 +3976,10 @@
     </row>
     <row r="17" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="61"/>
-      <c r="B17" s="88" t="s">
+      <c r="B17" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="89" t="s">
+      <c r="C17" s="81" t="s">
         <v>55</v>
       </c>
       <c r="D17" s="27">
@@ -3994,7 +3993,7 @@
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="I17" s="44"/>
@@ -4105,10 +4104,10 @@
     </row>
     <row r="18" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="60"/>
-      <c r="B18" s="88" t="s">
+      <c r="B18" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="89" t="s">
+      <c r="C18" s="81" t="s">
         <v>56</v>
       </c>
       <c r="D18" s="27">
@@ -4122,7 +4121,7 @@
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="I18" s="44"/>
@@ -4233,16 +4232,16 @@
     </row>
     <row r="19" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="60"/>
-      <c r="B19" s="88" t="s">
+      <c r="B19" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="89" t="s">
+      <c r="C19" s="81" t="s">
         <v>46</v>
       </c>
       <c r="D19" s="27">
         <v>0</v>
       </c>
-      <c r="E19" s="94">
+      <c r="E19" s="86">
         <v>43374</v>
       </c>
       <c r="F19" s="68">
@@ -4358,10 +4357,10 @@
     </row>
     <row r="20" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="60"/>
-      <c r="B20" s="88" t="s">
+      <c r="B20" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="89" t="s">
+      <c r="C20" s="81" t="s">
         <v>43</v>
       </c>
       <c r="D20" s="27">
@@ -4377,7 +4376,7 @@
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="I20" s="44"/>
@@ -4488,10 +4487,10 @@
     </row>
     <row r="21" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="60"/>
-      <c r="B21" s="88" t="s">
+      <c r="B21" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="89" t="s">
+      <c r="C21" s="81" t="s">
         <v>43</v>
       </c>
       <c r="D21" s="27">
@@ -4505,7 +4504,7 @@
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="I21" s="44"/>
@@ -4616,10 +4615,10 @@
     </row>
     <row r="22" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="60"/>
-      <c r="B22" s="88" t="s">
+      <c r="B22" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="89" t="s">
+      <c r="C22" s="81" t="s">
         <v>55</v>
       </c>
       <c r="D22" s="27">
@@ -4628,7 +4627,7 @@
       <c r="E22" s="68">
         <v>43376</v>
       </c>
-      <c r="F22" s="94">
+      <c r="F22" s="86">
         <v>43397</v>
       </c>
       <c r="G22" s="17"/>
@@ -4741,10 +4740,10 @@
     </row>
     <row r="23" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="60"/>
-      <c r="B23" s="88" t="s">
+      <c r="B23" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="89" t="s">
+      <c r="C23" s="81" t="s">
         <v>43</v>
       </c>
       <c r="D23" s="27">
@@ -4875,7 +4874,7 @@
       <c r="F24" s="31"/>
       <c r="G24" s="17"/>
       <c r="H24" s="17" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I24" s="44"/>
@@ -4986,10 +4985,10 @@
     </row>
     <row r="25" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="60"/>
-      <c r="B25" s="90" t="s">
+      <c r="B25" s="82" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="91" t="s">
+      <c r="C25" s="83" t="s">
         <v>46</v>
       </c>
       <c r="D25" s="32">
@@ -4998,7 +4997,7 @@
       <c r="E25" s="69">
         <v>43387</v>
       </c>
-      <c r="F25" s="95">
+      <c r="F25" s="87">
         <v>43401</v>
       </c>
       <c r="G25" s="17"/>
@@ -5111,10 +5110,10 @@
     </row>
     <row r="26" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="60"/>
-      <c r="B26" s="90" t="s">
+      <c r="B26" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="91" t="s">
+      <c r="C26" s="83" t="s">
         <v>46</v>
       </c>
       <c r="D26" s="32">
@@ -5238,10 +5237,10 @@
       <c r="A27" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="90" t="s">
+      <c r="B27" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="91" t="s">
+      <c r="C27" s="83" t="s">
         <v>45</v>
       </c>
       <c r="D27" s="32">
@@ -5250,12 +5249,12 @@
       <c r="E27" s="69">
         <v>43388</v>
       </c>
-      <c r="F27" s="95">
+      <c r="F27" s="87">
         <v>43409</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>22</v>
       </c>
       <c r="I27" s="44"/>
@@ -5366,10 +5365,10 @@
     </row>
     <row r="28" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="60"/>
-      <c r="B28" s="90" t="s">
+      <c r="B28" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="91" t="s">
+      <c r="C28" s="83" t="s">
         <v>56</v>
       </c>
       <c r="D28" s="32">
@@ -5383,7 +5382,7 @@
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44</v>
       </c>
       <c r="I28" s="44"/>
@@ -5494,10 +5493,10 @@
     </row>
     <row r="29" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="60"/>
-      <c r="B29" s="90" t="s">
+      <c r="B29" s="82" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="91" t="s">
+      <c r="C29" s="83" t="s">
         <v>56</v>
       </c>
       <c r="D29" s="32">
@@ -5619,10 +5618,10 @@
     </row>
     <row r="30" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="60"/>
-      <c r="B30" s="90" t="s">
+      <c r="B30" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="91" t="s">
+      <c r="C30" s="83" t="s">
         <v>43</v>
       </c>
       <c r="D30" s="32">
@@ -5636,7 +5635,7 @@
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>29</v>
       </c>
       <c r="I30" s="44"/>
@@ -5747,10 +5746,10 @@
     </row>
     <row r="31" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="60"/>
-      <c r="B31" s="90" t="s">
+      <c r="B31" s="82" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="91" t="s">
+      <c r="C31" s="83" t="s">
         <v>45</v>
       </c>
       <c r="D31" s="32">
@@ -5872,10 +5871,10 @@
     </row>
     <row r="32" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="60"/>
-      <c r="B32" s="90" t="s">
+      <c r="B32" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="91" t="s">
+      <c r="C32" s="83" t="s">
         <v>45</v>
       </c>
       <c r="D32" s="32">
@@ -5997,10 +5996,10 @@
     </row>
     <row r="33" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="60"/>
-      <c r="B33" s="90" t="s">
+      <c r="B33" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="91" t="s">
+      <c r="C33" s="83" t="s">
         <v>45</v>
       </c>
       <c r="D33" s="32">
@@ -6122,10 +6121,10 @@
     </row>
     <row r="34" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="60"/>
-      <c r="B34" s="90" t="s">
+      <c r="B34" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="91" t="s">
+      <c r="C34" s="83" t="s">
         <v>45</v>
       </c>
       <c r="D34" s="32">
@@ -6247,10 +6246,10 @@
     </row>
     <row r="35" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="60"/>
-      <c r="B35" s="90" t="s">
+      <c r="B35" s="82" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="91" t="s">
+      <c r="C35" s="83" t="s">
         <v>58</v>
       </c>
       <c r="D35" s="32">
@@ -6259,12 +6258,12 @@
       <c r="E35" s="69">
         <v>43424</v>
       </c>
-      <c r="F35" s="95">
+      <c r="F35" s="87">
         <v>43431</v>
       </c>
       <c r="G35" s="17"/>
       <c r="H35" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="I35" s="44"/>
@@ -6375,10 +6374,10 @@
     </row>
     <row r="36" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="60"/>
-      <c r="B36" s="90" t="s">
+      <c r="B36" s="82" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="91" t="s">
+      <c r="C36" s="83" t="s">
         <v>43</v>
       </c>
       <c r="D36" s="32">
@@ -6392,7 +6391,7 @@
       </c>
       <c r="G36" s="17"/>
       <c r="H36" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="I36" s="44"/>
@@ -6512,7 +6511,7 @@
       <c r="F37" s="36"/>
       <c r="G37" s="17"/>
       <c r="H37" s="17" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I37" s="44"/>
@@ -6625,10 +6624,10 @@
       <c r="A38" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="92" t="s">
+      <c r="B38" s="84" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="93" t="s">
+      <c r="C38" s="85" t="s">
         <v>46</v>
       </c>
       <c r="D38" s="37">
@@ -6642,7 +6641,7 @@
       </c>
       <c r="G38" s="17"/>
       <c r="H38" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="I38" s="44"/>
@@ -6753,10 +6752,10 @@
     </row>
     <row r="39" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="60"/>
-      <c r="B39" s="92" t="s">
+      <c r="B39" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="93" t="s">
+      <c r="C39" s="85" t="s">
         <v>43</v>
       </c>
       <c r="D39" s="37">
@@ -6770,7 +6769,7 @@
       </c>
       <c r="G39" s="17"/>
       <c r="H39" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="I39" s="44"/>
@@ -6881,10 +6880,10 @@
     </row>
     <row r="40" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="60"/>
-      <c r="B40" s="92" t="s">
+      <c r="B40" s="84" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="93" t="s">
+      <c r="C40" s="85" t="s">
         <v>45</v>
       </c>
       <c r="D40" s="37">
@@ -6898,7 +6897,7 @@
       </c>
       <c r="G40" s="17"/>
       <c r="H40" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="I40" s="44"/>
@@ -7009,10 +7008,10 @@
     </row>
     <row r="41" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="60"/>
-      <c r="B41" s="92" t="s">
+      <c r="B41" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="C41" s="93" t="s">
+      <c r="C41" s="85" t="s">
         <v>45</v>
       </c>
       <c r="D41" s="37">
@@ -7026,7 +7025,7 @@
       </c>
       <c r="G41" s="17"/>
       <c r="H41" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="I41" s="44"/>
@@ -7137,10 +7136,10 @@
     </row>
     <row r="42" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="60"/>
-      <c r="B42" s="92" t="s">
+      <c r="B42" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="93" t="s">
+      <c r="C42" s="85" t="s">
         <v>43</v>
       </c>
       <c r="D42" s="37">
@@ -7154,7 +7153,7 @@
       </c>
       <c r="G42" s="17"/>
       <c r="H42" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="I42" s="44"/>
@@ -7272,7 +7271,7 @@
       <c r="F43" s="71"/>
       <c r="G43" s="17"/>
       <c r="H43" s="17" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I43" s="44"/>
@@ -7394,7 +7393,7 @@
       <c r="F44" s="42"/>
       <c r="G44" s="43"/>
       <c r="H44" s="43" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I44" s="46"/>
@@ -7518,6 +7517,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="CV4:DB4"/>
     <mergeCell ref="DC4:DI4"/>
     <mergeCell ref="BM4:BS4"/>
@@ -7525,18 +7536,6 @@
     <mergeCell ref="CA4:CG4"/>
     <mergeCell ref="CH4:CN4"/>
     <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D44">
     <cfRule type="dataBar" priority="37">
@@ -7566,7 +7565,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="E4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="E4">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
@@ -7602,7 +7601,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
@@ -7695,10 +7694,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="A2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="A13" r:id="rId1"/>
+    <hyperlink ref="A10" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>